<commit_message>
First working version of Telegram bot
</commit_message>
<xml_diff>
--- a/prices.xlsx
+++ b/prices.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mohammedemad/phone_price_bot/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0220F5A1-1054-6C40-849E-372BFF270B49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47897CB6-3971-CB4D-A9E2-D046D9815325}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17820" xr2:uid="{E46CB62F-FE53-A44C-937C-084064EC55F5}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17460" xr2:uid="{E46CB62F-FE53-A44C-937C-084064EC55F5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="178">
   <si>
     <t>الاسم (name)</t>
   </si>
@@ -85,18 +85,12 @@
     <t>4/128GB</t>
   </si>
   <si>
-    <t>Galaxy Z Fold 6</t>
-  </si>
-  <si>
     <t>12/512GB</t>
   </si>
   <si>
     <t>Galaxy S25 Ultra - Jet Black</t>
   </si>
   <si>
-    <t>Galaxy S25 Plus</t>
-  </si>
-  <si>
     <t>8/512GB</t>
   </si>
   <si>
@@ -211,18 +205,6 @@
     <t>Realme Note 60X</t>
   </si>
   <si>
-    <t>Honor Magic 7 Pro &amp; Watch + Pad X9</t>
-  </si>
-  <si>
-    <t>Honor 400 Pro &amp; watch</t>
-  </si>
-  <si>
-    <t>Honor 400 &amp; Buds</t>
-  </si>
-  <si>
-    <t>Honor 200 &amp; Buds</t>
-  </si>
-  <si>
     <t>Mi 15</t>
   </si>
   <si>
@@ -370,81 +352,12 @@
     <t>Huawei FreeBuds SE3</t>
   </si>
   <si>
-    <t>Infinix XPad 10.95inc Wi-Fi</t>
-  </si>
-  <si>
-    <t>Infinix XPad 10.95inc SIM</t>
-  </si>
-  <si>
-    <t>Tecno MegaPad 10.1inc SIM</t>
-  </si>
-  <si>
-    <t>Tecno MegaPad 11.1inc SIM</t>
-  </si>
-  <si>
-    <t>Blackview MEGA 2 11.79inc SIM</t>
-  </si>
-  <si>
-    <t>BlackView Tab 60 Pro 10.1inc SIM</t>
-  </si>
-  <si>
-    <t>BlackView Tab A6 Kids 10.1inc Wi-Fi</t>
-  </si>
-  <si>
-    <t>BlackView Tab 60 8.68 inc Wi-Fi</t>
-  </si>
-  <si>
     <t>8/128GE</t>
   </si>
   <si>
     <t xml:space="preserve">4/256GB </t>
   </si>
   <si>
-    <t>Huawei MatePad SE - Wi-Fi App Gallery</t>
-  </si>
-  <si>
-    <t>Huawei Matepad 11.5 - Wi-Fi App Gallery</t>
-  </si>
-  <si>
-    <t>Huawei MatePad Pro - Wi-Fi App Gallery</t>
-  </si>
-  <si>
-    <t>Xiaomi Pad 7 11.2inc Wi-Fi</t>
-  </si>
-  <si>
-    <t>Xiaomi Pad 7 Pro 11.2inc Wi-Fi</t>
-  </si>
-  <si>
-    <t>Redmi Pad SE 11.Oinc Wi-Fi</t>
-  </si>
-  <si>
-    <t>Redmi Pad Pro 12.1inc Wi-Fi</t>
-  </si>
-  <si>
-    <t>Redmi Pad Pro 5G 12.1 inc SIM</t>
-  </si>
-  <si>
-    <t>honor MagicPad 2 12.3inc Wi-Fi</t>
-  </si>
-  <si>
-    <t>honor Pad V9 11.5inc Wi-Fi</t>
-  </si>
-  <si>
-    <t>honor Pad 9 12.1inc Wi-Fi</t>
-  </si>
-  <si>
-    <t>honor Pad X9a 11.5inc Wi-Fi</t>
-  </si>
-  <si>
-    <t>honor Pad X9 11.5inc Wi-Fi</t>
-  </si>
-  <si>
-    <t>honor Pad X8a 11.0incWi-Fi</t>
-  </si>
-  <si>
-    <t>honor Pad X8a Kids 11.0incWi-Fi</t>
-  </si>
-  <si>
     <t>iPhone 16 Pro Max</t>
   </si>
   <si>
@@ -454,9 +367,6 @@
     <t>2,230,000 IQD</t>
   </si>
   <si>
-    <t>iPhone 16 Pro Max نسخة الدبل سيم كارت</t>
-  </si>
-  <si>
     <t>512GB</t>
   </si>
   <si>
@@ -475,9 +385,6 @@
     <t>1,925,000 IQD</t>
   </si>
   <si>
-    <t>iPhone 16 Plus نسخة الشرق الاوسط</t>
-  </si>
-  <si>
     <t>1,335,000 QD</t>
   </si>
   <si>
@@ -487,82 +394,184 @@
     <t>1,185,000 QD</t>
   </si>
   <si>
-    <t>نسخة الشرق الاوسط iPhone 16</t>
-  </si>
-  <si>
     <t>X</t>
   </si>
   <si>
     <t>1,035,000 IQD</t>
   </si>
   <si>
-    <t>نسئة الشرق الاوسط iPhone 15</t>
-  </si>
-  <si>
-    <t>نسخة الشرق الاوسط iPhone 14</t>
-  </si>
-  <si>
-    <t>نسخة الشرق الاوسط iPhone 13</t>
-  </si>
-  <si>
     <t>590,000 IQD</t>
   </si>
   <si>
-    <t>iPad Pro 13-inch M4 WiFi</t>
-  </si>
-  <si>
-    <t>(256GB</t>
-  </si>
-  <si>
     <t>1,620,000 IQD</t>
   </si>
   <si>
-    <t>(512GB</t>
-  </si>
-  <si>
     <t>1,890,000 QD</t>
   </si>
   <si>
-    <t>2TB</t>
-  </si>
-  <si>
     <t>2,650,000 IQD</t>
   </si>
   <si>
-    <t>iPad Pro 11-inch M4 WiFi</t>
-  </si>
-  <si>
     <t>1,320,000 QD</t>
   </si>
   <si>
     <t>1,590,000 IQD</t>
   </si>
   <si>
-    <t>iPad Air 7 M3 Chip 13-inch</t>
-  </si>
-  <si>
     <t>1,090,000 IQD</t>
   </si>
   <si>
     <t>1,225,000 IQD</t>
   </si>
   <si>
-    <t>iPad Air 7 M3 Chip 11-inch</t>
-  </si>
-  <si>
     <t>930,000 IQD</t>
   </si>
   <si>
     <t>790,000 IQD</t>
   </si>
   <si>
-    <t>iPad 1l-inch A16 Chip</t>
-  </si>
-  <si>
     <t>500,000 IQD</t>
   </si>
   <si>
     <t>600,000 IQD</t>
+  </si>
+  <si>
+    <t>Galaxy Z Fold6</t>
+  </si>
+  <si>
+    <t>Galaxy S25+</t>
+  </si>
+  <si>
+    <t>Honor Magic7 Pro</t>
+  </si>
+  <si>
+    <t>Honor 400 Pro</t>
+  </si>
+  <si>
+    <t>Honor 400</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Honor 200 </t>
+  </si>
+  <si>
+    <t>11-inch-M3-128GB</t>
+  </si>
+  <si>
+    <t>11-inch-M3-256GB</t>
+  </si>
+  <si>
+    <t>13-inch-M3-256GB</t>
+  </si>
+  <si>
+    <t>13-inch-M3-128GB</t>
+  </si>
+  <si>
+    <t>11-inch -M4 WiFi-512GB</t>
+  </si>
+  <si>
+    <t>11-inch -M4 WiFi-256GB</t>
+  </si>
+  <si>
+    <t>13-inch -M4 WiFi-2TB</t>
+  </si>
+  <si>
+    <t>13-inch -M4 WiFi-512GB</t>
+  </si>
+  <si>
+    <t>iPad 11</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> iPhone 13</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> iPhone 14</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> iPhone 15</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> iPhone 16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">iPhone 16 Plus </t>
+  </si>
+  <si>
+    <t xml:space="preserve">iPhone 16 Pro Max  الدبل سيم </t>
+  </si>
+  <si>
+    <t xml:space="preserve">honor Pad X8a </t>
+  </si>
+  <si>
+    <t xml:space="preserve">honor Pad X9 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">honor Pad X9a </t>
+  </si>
+  <si>
+    <t xml:space="preserve">honor Pad 9 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">honor Pad V9 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">honor MagicPad 2 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Redmi Pad Pro 5G </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Redmi Pad Pro </t>
+  </si>
+  <si>
+    <t>Redmi Pad SE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Xiaomi Pad 7 Pro </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Xiaomi Pad 7 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Huawei MatePad Pro </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Huawei Matepad 11.5 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Huawei MatePad SE </t>
+  </si>
+  <si>
+    <t xml:space="preserve">BlackView Tab 60 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">BlackView Tab A6 Kids </t>
+  </si>
+  <si>
+    <t xml:space="preserve">BlackView Tab 60 Pro </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Blackview MEGA 2 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tecno MegaPad </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Infinix XPad </t>
+  </si>
+  <si>
+    <t>M4 WiFi-256GB</t>
+  </si>
+  <si>
+    <t>iPad Air 7 11"</t>
+  </si>
+  <si>
+    <t>iPad Air 7 13"</t>
+  </si>
+  <si>
+    <t>iPad Pro 11"</t>
+  </si>
+  <si>
+    <t>iPad Pro 13"</t>
   </si>
 </sst>
 </file>
@@ -946,15 +955,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2A32F0D-D5B4-E741-9E04-6E6BE25344F9}">
   <dimension ref="A1:C169"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A133" workbookViewId="0">
-      <selection activeCell="D156" sqref="D156"/>
+    <sheetView tabSelected="1" topLeftCell="A144" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="E153" sqref="E153"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="31.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.83203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.5" customWidth="1"/>
   </cols>
@@ -967,12 +976,12 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>15</v>
+        <v>132</v>
       </c>
       <c r="B2" s="3">
         <v>1779000</v>
@@ -983,13 +992,13 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>15</v>
+        <v>132</v>
       </c>
       <c r="B3" s="3">
         <v>2625000</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -1005,7 +1014,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B5" s="3">
         <v>1350000</v>
@@ -1016,7 +1025,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>18</v>
+        <v>133</v>
       </c>
       <c r="B6" s="3">
         <v>1150000</v>
@@ -1027,13 +1036,13 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>18</v>
+        <v>133</v>
       </c>
       <c r="B7" s="3">
         <v>1250000</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -1066,7 +1075,7 @@
         <v>920000</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
@@ -1099,7 +1108,7 @@
         <v>387000</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
@@ -1121,7 +1130,7 @@
         <v>295000</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
@@ -1154,7 +1163,7 @@
         <v>183000</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
@@ -1176,7 +1185,7 @@
         <v>102000</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
@@ -1198,89 +1207,89 @@
         <v>132000</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B23" s="4">
         <v>80000</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B24" s="4">
         <v>108000</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B25" s="4">
         <v>159000</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
-        <v>57</v>
+        <v>134</v>
       </c>
       <c r="B26" s="4">
         <v>1330000</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
-        <v>58</v>
+        <v>135</v>
       </c>
       <c r="B27" s="4">
         <v>812000</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
-        <v>59</v>
+        <v>136</v>
       </c>
       <c r="B28" s="4">
         <v>490000</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
-        <v>60</v>
+        <v>137</v>
       </c>
       <c r="B29" s="4">
         <v>475000</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B30" s="4">
         <v>352000</v>
@@ -1291,7 +1300,7 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B31" s="4">
         <v>328000</v>
@@ -1302,7 +1311,7 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B32" s="4">
         <v>320000</v>
@@ -1313,7 +1322,7 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B33" s="4">
         <v>260000</v>
@@ -1324,18 +1333,18 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B34" s="4">
         <v>290000</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B35" s="4">
         <v>180000</v>
@@ -1346,40 +1355,40 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B36" s="4">
         <v>123000</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B37" s="4">
         <v>137000</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B38" s="4">
         <v>98000</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B39" s="4">
         <v>108000</v>
@@ -1390,7 +1399,7 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B40" s="4">
         <v>480000</v>
@@ -1401,7 +1410,7 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B41" s="4">
         <v>348000</v>
@@ -1412,7 +1421,7 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B42" s="4">
         <v>320000</v>
@@ -1423,7 +1432,7 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B43" s="4">
         <v>290000</v>
@@ -1434,7 +1443,7 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B44" s="4">
         <v>255000</v>
@@ -1445,7 +1454,7 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B45" s="4">
         <v>250000</v>
@@ -1456,7 +1465,7 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B46" s="4">
         <v>189000</v>
@@ -1467,7 +1476,7 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B47" s="4">
         <v>180000</v>
@@ -1478,7 +1487,7 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B48" s="4">
         <v>138000</v>
@@ -1489,7 +1498,7 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B49" s="4">
         <v>144000</v>
@@ -1500,7 +1509,7 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B50" s="4">
         <v>98000</v>
@@ -1511,7 +1520,7 @@
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B51" s="4">
         <v>116000</v>
@@ -1522,40 +1531,40 @@
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B52" s="4">
         <v>1258000</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B53" s="4">
         <v>825000</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B54" s="4">
         <v>500000</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B55" s="4">
         <v>462000</v>
@@ -1566,18 +1575,18 @@
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B56" s="4">
         <v>595000</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B57" s="4">
         <v>237000</v>
@@ -1588,29 +1597,29 @@
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B58" s="4">
         <v>284000</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B59" s="4">
         <v>168000</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B60" s="4">
         <v>199000</v>
@@ -1621,18 +1630,18 @@
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B61" s="4">
         <v>157000</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A62" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B62" s="4">
         <v>193000</v>
@@ -1643,18 +1652,18 @@
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A63" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B63" s="4">
         <v>105000</v>
       </c>
       <c r="C63" s="4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A64" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B64" s="4">
         <v>120000</v>
@@ -1665,7 +1674,7 @@
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A65" s="2" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="B65" s="4">
         <v>980000</v>
@@ -1676,7 +1685,7 @@
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A66" s="2" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="B66" s="4">
         <v>511000</v>
@@ -1687,40 +1696,40 @@
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A67" s="2" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="B67" s="4">
         <v>563000</v>
       </c>
       <c r="C67" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A68" s="2" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="B68" s="4">
         <v>738000</v>
       </c>
       <c r="C68" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A69" s="2" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="B69" s="4">
         <v>800000</v>
       </c>
       <c r="C69" s="4" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A70" s="2" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="B70" s="4">
         <v>222000</v>
@@ -1731,7 +1740,7 @@
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A71" s="2" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="B71" s="4">
         <v>275000</v>
@@ -1742,7 +1751,7 @@
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A72" s="2" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="B72" s="4">
         <v>307000</v>
@@ -1753,40 +1762,40 @@
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A73" s="2" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="B73" s="4">
         <v>370000</v>
       </c>
       <c r="C73" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A74" s="2" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="B74" s="4">
         <v>418000</v>
       </c>
       <c r="C74" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A75" s="2" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="B75" s="4">
         <v>501000</v>
       </c>
       <c r="C75" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A76" s="2" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="B76" s="4">
         <v>164000</v>
@@ -1797,7 +1806,7 @@
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A77" s="2" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="B77" s="4">
         <v>120000</v>
@@ -1808,7 +1817,7 @@
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A78" s="2" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="B78" s="4">
         <v>148000</v>
@@ -1819,7 +1828,7 @@
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A79" s="2" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="B79" s="4">
         <v>88000</v>
@@ -1830,7 +1839,7 @@
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A80" s="2" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="B80" s="4">
         <v>103000</v>
@@ -1841,51 +1850,51 @@
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A81" s="2" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="B81" s="4">
         <v>926000</v>
       </c>
       <c r="C81" s="4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A82" s="2" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="B82" s="4">
         <v>677000</v>
       </c>
       <c r="C82" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A83" s="2" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="B83" s="4">
         <v>664000</v>
       </c>
       <c r="C83" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A84" s="2" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="B84" s="4">
         <v>360000</v>
       </c>
       <c r="C84" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A85" s="2" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="B85" s="4">
         <v>415000</v>
@@ -1896,29 +1905,29 @@
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A86" s="2" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="B86" s="4">
         <v>459000</v>
       </c>
       <c r="C86" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A87" s="2" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="B87" s="4">
         <v>437000</v>
       </c>
       <c r="C87" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A88" s="2" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B88" s="4">
         <v>262000</v>
@@ -1929,18 +1938,18 @@
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A89" s="2" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="B89" s="4">
         <v>303000</v>
       </c>
       <c r="C89" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A90" s="2" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="B90" s="4">
         <v>147000</v>
@@ -1951,7 +1960,7 @@
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A91" s="2" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="B91" s="4">
         <v>105000</v>
@@ -1962,7 +1971,7 @@
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A92" s="2" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="B92" s="4">
         <v>395000</v>
@@ -1973,18 +1982,18 @@
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A93" s="2" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="B93" s="4">
         <v>314000</v>
       </c>
       <c r="C93" s="4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A94" s="2" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="B94" s="4">
         <v>407000</v>
@@ -1995,18 +2004,18 @@
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A95" s="2" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="B95" s="4">
         <v>473000</v>
       </c>
       <c r="C95" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A96" s="2" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="B96" s="4">
         <v>250000</v>
@@ -2017,7 +2026,7 @@
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A97" s="2" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="B97" s="4">
         <v>285000</v>
@@ -2028,7 +2037,7 @@
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A98" s="2" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="B98" s="4">
         <v>305000</v>
@@ -2039,7 +2048,7 @@
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A99" s="2" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="B99" s="4">
         <v>465000</v>
@@ -2050,18 +2059,18 @@
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A100" s="2" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="B100" s="4">
         <v>158000</v>
       </c>
       <c r="C100" s="4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A101" s="2" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="B101" s="4">
         <v>137000</v>
@@ -2072,7 +2081,7 @@
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A102" s="2" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="B102" s="4">
         <v>199000</v>
@@ -2083,7 +2092,7 @@
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A103" s="2" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="B103" s="4">
         <v>224000</v>
@@ -2094,7 +2103,7 @@
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A104" s="2" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="B104" s="4">
         <v>97000</v>
@@ -2105,7 +2114,7 @@
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A105" s="2" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="B105" s="4">
         <v>116000</v>
@@ -2116,172 +2125,172 @@
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A106" s="2" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="B106" s="4">
         <v>238000</v>
       </c>
       <c r="C106" s="4" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A107" s="2" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="B107" s="4">
         <v>373000</v>
       </c>
       <c r="C107" s="4" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A108" s="2" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="B108" s="4">
         <v>493000</v>
       </c>
       <c r="C108" s="4" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A109" s="2" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="B109" s="4">
         <v>433000</v>
       </c>
       <c r="C109" s="4" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A110" s="2" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="B110" s="4">
         <v>178000</v>
       </c>
       <c r="C110" s="4" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A111" s="2" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="B111" s="4">
         <v>283000</v>
       </c>
       <c r="C111" s="4" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A112" s="2" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="B112" s="4">
         <v>140000</v>
       </c>
       <c r="C112" s="4" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A113" s="2" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="B113" s="4">
         <v>160000</v>
       </c>
       <c r="C113" s="4" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A114" s="2" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="B114" s="4">
         <v>190000</v>
       </c>
       <c r="C114" s="4" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A115" s="2" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="B115" s="4">
         <v>223000</v>
       </c>
       <c r="C115" s="4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A116" s="2" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="B116" s="4">
         <v>185000</v>
       </c>
       <c r="C116" s="4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A117" s="2" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="B117" s="4">
         <v>126000</v>
       </c>
       <c r="C117" s="4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A118" s="2" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="B118" s="4">
         <v>133000</v>
       </c>
       <c r="C118" s="4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A119" s="2" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="B119" s="4">
         <v>88000</v>
       </c>
       <c r="C119" s="4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A120" s="2" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="B120" s="4">
         <v>49000</v>
       </c>
       <c r="C120" s="4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A121" s="2" t="s">
-        <v>110</v>
+        <v>172</v>
       </c>
       <c r="B121" s="4">
         <v>193000</v>
@@ -2292,7 +2301,7 @@
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A122" s="2" t="s">
-        <v>111</v>
+        <v>172</v>
       </c>
       <c r="B122" s="4">
         <v>233000</v>
@@ -2303,7 +2312,7 @@
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A123" s="2" t="s">
-        <v>112</v>
+        <v>171</v>
       </c>
       <c r="B123" s="4">
         <v>165000</v>
@@ -2314,18 +2323,18 @@
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A124" s="2" t="s">
-        <v>112</v>
+        <v>171</v>
       </c>
       <c r="B124" s="4">
         <v>195000</v>
       </c>
       <c r="C124" s="4" t="s">
-        <v>119</v>
+        <v>105</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A125" s="2" t="s">
-        <v>113</v>
+        <v>171</v>
       </c>
       <c r="B125" s="4">
         <v>235000</v>
@@ -2336,7 +2345,7 @@
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A126" s="2" t="s">
-        <v>114</v>
+        <v>170</v>
       </c>
       <c r="B126" s="4">
         <v>198000</v>
@@ -2347,18 +2356,18 @@
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A127" s="2" t="s">
-        <v>115</v>
+        <v>169</v>
       </c>
       <c r="B127" s="4">
         <v>160000</v>
       </c>
       <c r="C127" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A128" s="2" t="s">
-        <v>116</v>
+        <v>168</v>
       </c>
       <c r="B128" s="4">
         <v>115000</v>
@@ -2369,7 +2378,7 @@
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A129" s="2" t="s">
-        <v>117</v>
+        <v>167</v>
       </c>
       <c r="B129" s="4">
         <v>110000</v>
@@ -2380,18 +2389,18 @@
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A130" s="2" t="s">
-        <v>120</v>
+        <v>166</v>
       </c>
       <c r="B130" s="4">
         <v>283000</v>
       </c>
       <c r="C130" s="4" t="s">
-        <v>118</v>
+        <v>104</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A131" s="2" t="s">
-        <v>121</v>
+        <v>165</v>
       </c>
       <c r="B131" s="4">
         <v>435000</v>
@@ -2402,18 +2411,18 @@
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A132" s="2" t="s">
-        <v>122</v>
+        <v>164</v>
       </c>
       <c r="B132" s="4">
         <v>1183000</v>
       </c>
       <c r="C132" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A133" s="2" t="s">
-        <v>123</v>
+        <v>163</v>
       </c>
       <c r="B133" s="4">
         <v>465000</v>
@@ -2424,7 +2433,7 @@
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A134" s="2" t="s">
-        <v>123</v>
+        <v>163</v>
       </c>
       <c r="B134" s="4">
         <v>507000</v>
@@ -2435,18 +2444,18 @@
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A135" s="2" t="s">
-        <v>124</v>
+        <v>162</v>
       </c>
       <c r="B135" s="4">
         <v>665000</v>
       </c>
       <c r="C135" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A136" s="2" t="s">
-        <v>125</v>
+        <v>161</v>
       </c>
       <c r="B136" s="4">
         <v>229000</v>
@@ -2457,7 +2466,7 @@
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A137" s="2" t="s">
-        <v>126</v>
+        <v>160</v>
       </c>
       <c r="B137" s="4">
         <v>320000</v>
@@ -2468,7 +2477,7 @@
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A138" s="2" t="s">
-        <v>127</v>
+        <v>159</v>
       </c>
       <c r="B138" s="4">
         <v>391000</v>
@@ -2479,7 +2488,7 @@
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A139" s="2" t="s">
-        <v>128</v>
+        <v>158</v>
       </c>
       <c r="B139" s="4">
         <v>813000</v>
@@ -2490,7 +2499,7 @@
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A140" s="2" t="s">
-        <v>129</v>
+        <v>157</v>
       </c>
       <c r="B140" s="4">
         <v>635000</v>
@@ -2501,7 +2510,7 @@
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A141" s="2" t="s">
-        <v>130</v>
+        <v>156</v>
       </c>
       <c r="B141" s="4">
         <v>342000</v>
@@ -2512,7 +2521,7 @@
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A142" s="2" t="s">
-        <v>131</v>
+        <v>155</v>
       </c>
       <c r="B142" s="4">
         <v>265000</v>
@@ -2523,7 +2532,7 @@
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A143" s="2" t="s">
-        <v>132</v>
+        <v>154</v>
       </c>
       <c r="B143" s="4">
         <v>213000</v>
@@ -2534,7 +2543,7 @@
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A144" s="2" t="s">
-        <v>133</v>
+        <v>153</v>
       </c>
       <c r="B144" s="4">
         <v>185000</v>
@@ -2545,7 +2554,7 @@
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A145" s="2" t="s">
-        <v>134</v>
+        <v>153</v>
       </c>
       <c r="B145" s="4">
         <v>185000</v>
@@ -2556,255 +2565,255 @@
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A146" s="2" t="s">
-        <v>135</v>
+        <v>106</v>
       </c>
       <c r="B146" s="4" t="s">
-        <v>137</v>
+        <v>108</v>
       </c>
       <c r="C146" s="4" t="s">
-        <v>136</v>
+        <v>107</v>
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A147" s="2" t="s">
-        <v>138</v>
+        <v>152</v>
       </c>
       <c r="B147" s="4" t="s">
-        <v>140</v>
+        <v>110</v>
       </c>
       <c r="C147" s="4" t="s">
-        <v>139</v>
+        <v>109</v>
       </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A148" s="2" t="s">
-        <v>135</v>
+        <v>106</v>
       </c>
       <c r="B148" s="4" t="s">
-        <v>142</v>
+        <v>112</v>
       </c>
       <c r="C148" s="4" t="s">
-        <v>141</v>
+        <v>111</v>
       </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A149" s="2" t="s">
-        <v>135</v>
+        <v>106</v>
       </c>
       <c r="B149" s="4" t="s">
-        <v>143</v>
+        <v>113</v>
       </c>
       <c r="C149" s="4" t="s">
-        <v>141</v>
+        <v>111</v>
       </c>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A150" s="2" t="s">
-        <v>135</v>
+        <v>106</v>
       </c>
       <c r="B150" s="4" t="s">
-        <v>144</v>
+        <v>114</v>
       </c>
       <c r="C150" s="4" t="s">
-        <v>139</v>
+        <v>109</v>
       </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A151" s="2" t="s">
-        <v>145</v>
+        <v>151</v>
       </c>
       <c r="B151" s="4" t="s">
-        <v>146</v>
+        <v>115</v>
       </c>
       <c r="C151" s="4" t="s">
-        <v>141</v>
+        <v>111</v>
       </c>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A152" s="2" t="s">
-        <v>145</v>
+        <v>151</v>
       </c>
       <c r="B152" s="4" t="s">
-        <v>148</v>
+        <v>117</v>
       </c>
       <c r="C152" s="4" t="s">
-        <v>147</v>
+        <v>116</v>
       </c>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A153" s="6" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B153" s="4" t="s">
-        <v>150</v>
+        <v>118</v>
       </c>
       <c r="C153" s="4" t="s">
-        <v>141</v>
+        <v>111</v>
       </c>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A154" s="6" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B154" s="4" t="s">
-        <v>151</v>
+        <v>119</v>
       </c>
       <c r="C154" s="4" t="s">
-        <v>147</v>
+        <v>116</v>
       </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A155" s="6" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="B155" s="4" t="s">
-        <v>150</v>
+        <v>118</v>
       </c>
       <c r="C155" s="4" t="s">
-        <v>147</v>
+        <v>116</v>
       </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A156" s="6" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="B156" s="4" t="s">
-        <v>150</v>
+        <v>118</v>
       </c>
       <c r="C156" s="4" t="s">
-        <v>147</v>
+        <v>116</v>
       </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A157" s="6" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="B157" s="4" t="s">
-        <v>155</v>
+        <v>120</v>
       </c>
       <c r="C157" s="4" t="s">
-        <v>147</v>
+        <v>116</v>
       </c>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A158" s="6" t="s">
-        <v>156</v>
+        <v>177</v>
       </c>
       <c r="B158" s="4" t="s">
-        <v>158</v>
+        <v>121</v>
       </c>
       <c r="C158" s="4" t="s">
-        <v>157</v>
+        <v>173</v>
       </c>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A159" s="6" t="s">
-        <v>156</v>
+        <v>177</v>
       </c>
       <c r="B159" s="4" t="s">
-        <v>160</v>
+        <v>122</v>
       </c>
       <c r="C159" s="4" t="s">
-        <v>159</v>
+        <v>145</v>
       </c>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A160" s="6" t="s">
-        <v>156</v>
+        <v>177</v>
       </c>
       <c r="B160" s="4" t="s">
-        <v>162</v>
+        <v>123</v>
       </c>
       <c r="C160" s="4" t="s">
-        <v>161</v>
+        <v>144</v>
       </c>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A161" s="6" t="s">
-        <v>163</v>
+        <v>176</v>
       </c>
       <c r="B161" s="4" t="s">
-        <v>164</v>
+        <v>124</v>
       </c>
       <c r="C161" s="4" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A162" s="6" t="s">
-        <v>163</v>
+        <v>176</v>
       </c>
       <c r="B162" s="4" t="s">
-        <v>165</v>
+        <v>125</v>
       </c>
       <c r="C162" s="4" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A163" s="6" t="s">
-        <v>166</v>
+        <v>175</v>
       </c>
       <c r="B163" s="4" t="s">
-        <v>167</v>
+        <v>126</v>
       </c>
       <c r="C163" s="4" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A164" s="6" t="s">
-        <v>166</v>
+        <v>175</v>
       </c>
       <c r="B164" s="4" t="s">
-        <v>168</v>
+        <v>127</v>
       </c>
       <c r="C164" s="4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A165" s="6" t="s">
-        <v>169</v>
+        <v>174</v>
       </c>
       <c r="B165" s="4" t="s">
-        <v>170</v>
+        <v>128</v>
       </c>
       <c r="C165" s="4" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A166" s="6" t="s">
-        <v>169</v>
+        <v>174</v>
       </c>
       <c r="B166" s="4" t="s">
-        <v>171</v>
+        <v>129</v>
       </c>
       <c r="C166" s="4" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A167" s="6" t="s">
-        <v>172</v>
+        <v>146</v>
       </c>
       <c r="B167" s="4" t="s">
-        <v>173</v>
+        <v>130</v>
       </c>
       <c r="C167" s="4" t="s">
-        <v>147</v>
+        <v>116</v>
       </c>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A168" s="6" t="s">
-        <v>172</v>
+        <v>146</v>
       </c>
       <c r="B168" s="4" t="s">
-        <v>174</v>
+        <v>131</v>
       </c>
       <c r="C168" s="4" t="s">
-        <v>141</v>
+        <v>111</v>
       </c>
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.2">
@@ -2813,5 +2822,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>